<commit_message>
add entities and dto pojo classes
</commit_message>
<xml_diff>
--- a/doc/plan.xlsx
+++ b/doc/plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NAUKA_IT\JAVA\TruckPark-server_side\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C43DF6D1-0B77-49BF-B999-BD9B13ABEE20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB88BA9-A64B-471D-9C51-489C265373DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-9630" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Branch name</t>
   </si>
@@ -36,7 +36,13 @@
     <t>#100000</t>
   </si>
   <si>
-    <t>Create spring boot application schema</t>
+    <t>Initialization of application and beta database</t>
+  </si>
+  <si>
+    <t>#100001</t>
+  </si>
+  <si>
+    <t>Add entitites and dto objects</t>
   </si>
 </sst>
 </file>
@@ -354,16 +360,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.88671875" customWidth="1"/>
-    <col min="2" max="2" width="35.88671875" customWidth="1"/>
+    <col min="2" max="2" width="44.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -382,6 +388,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add some rercords to plan.xlsx
</commit_message>
<xml_diff>
--- a/doc/plan.xlsx
+++ b/doc/plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NAUKA_IT\JAVA\TruckPark-server_side\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB88BA9-A64B-471D-9C51-489C265373DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40A68492-10E2-4469-A9D3-8CD6F7EB7A96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Branch name</t>
   </si>
@@ -43,16 +43,40 @@
   </si>
   <si>
     <t>Add entitites and dto objects</t>
+  </si>
+  <si>
+    <t>#100002</t>
+  </si>
+  <si>
+    <t>Add mappers</t>
+  </si>
+  <si>
+    <t>#100003</t>
+  </si>
+  <si>
+    <t>Add simple Dao layers</t>
+  </si>
+  <si>
+    <t>#100004</t>
+  </si>
+  <si>
+    <t>Add Rest endpoints</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -360,19 +384,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" customWidth="1"/>
-    <col min="2" max="2" width="44.88671875" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="44.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -380,7 +404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -388,7 +412,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -396,7 +420,32 @@
         <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Create Rest endpoint for Trucks with required services #100003
</commit_message>
<xml_diff>
--- a/doc/plan.xlsx
+++ b/doc/plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NAUKA_IT\JAVA\TruckPark-server_side\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40A68492-10E2-4469-A9D3-8CD6F7EB7A96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E8D241-32BC-4DD4-9F19-910B33D46895}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Branch name</t>
   </si>
@@ -54,13 +54,7 @@
     <t>#100003</t>
   </si>
   <si>
-    <t>Add simple Dao layers</t>
-  </si>
-  <si>
-    <t>#100004</t>
-  </si>
-  <si>
-    <t>Add Rest endpoints</t>
+    <t>Add features for TruckWays, Trucks and Drivers</t>
   </si>
 </sst>
 </file>
@@ -384,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,14 +430,6 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Create functions for Mop and ExtendedMopData #100003
</commit_message>
<xml_diff>
--- a/doc/plan.xlsx
+++ b/doc/plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NAUKA_IT\JAVA\TruckPark-server_side\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E8D241-32BC-4DD4-9F19-910B33D46895}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87B165C4-2943-43DE-A756-2469FAD2BF7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Branch name</t>
   </si>
@@ -54,7 +54,13 @@
     <t>#100003</t>
   </si>
   <si>
-    <t>Add features for TruckWays, Trucks and Drivers</t>
+    <t>#100004</t>
+  </si>
+  <si>
+    <t>Add crud features for Trucks</t>
+  </si>
+  <si>
+    <t>Add crud features for Mop and extendedMop</t>
   </si>
 </sst>
 </file>
@@ -378,10 +384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,7 +433,15 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create functions for Driver #100003
</commit_message>
<xml_diff>
--- a/doc/plan.xlsx
+++ b/doc/plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NAUKA_IT\JAVA\TruckPark-server_side\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87B165C4-2943-43DE-A756-2469FAD2BF7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05145EC1-6B26-417B-A6BF-4D52AFB3F105}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,7 +60,7 @@
     <t>Add crud features for Trucks</t>
   </si>
   <si>
-    <t>Add crud features for Mop and extendedMop</t>
+    <t>Add crud basic features for objects</t>
   </si>
 </sst>
 </file>
@@ -390,13 +390,13 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="44.85546875" customWidth="1"/>
+    <col min="1" max="1" width="12.88671875" customWidth="1"/>
+    <col min="2" max="2" width="44.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -404,7 +404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -412,7 +412,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -420,7 +420,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -428,7 +428,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -436,7 +436,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Add angular module to project
</commit_message>
<xml_diff>
--- a/doc/plan.xlsx
+++ b/doc/plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NAUKA_IT\JAVA\TruckPark-server_side\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC8C850A-C8C5-47B4-91CD-A647661F75B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C692F8-21BA-47F6-A24C-0B468CE9382D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16320" yWindow="-9870" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Branch name</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>Add README.ME file</t>
+  </si>
+  <si>
+    <t>#100007</t>
+  </si>
+  <si>
+    <t>Add Angular front module to project</t>
   </si>
 </sst>
 </file>
@@ -396,19 +402,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" customWidth="1"/>
-    <col min="2" max="2" width="44.88671875" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="44.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -416,7 +422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -424,7 +430,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -432,7 +438,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -440,7 +446,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -448,7 +454,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -456,7 +462,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -464,12 +470,20 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Map component skeleton.
</commit_message>
<xml_diff>
--- a/doc/plan.xlsx
+++ b/doc/plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NAUKA_IT\JAVA\TruckPark-server_side\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C692F8-21BA-47F6-A24C-0B468CE9382D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EEAA433-38BA-4905-B88A-EE8C9A8B8172}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-9870" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Branch name</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>Add Angular front module to project</t>
+  </si>
+  <si>
+    <t>#100008</t>
+  </si>
+  <si>
+    <t>Create Map Component</t>
   </si>
 </sst>
 </file>
@@ -402,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,6 +492,14 @@
         <v>17</v>
       </c>
     </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add Ng Ant framework and integrate mops map with the rest of application
</commit_message>
<xml_diff>
--- a/doc/plan.xlsx
+++ b/doc/plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NAUKA_IT\JAVA\TruckPark-server_side\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EEAA433-38BA-4905-B88A-EE8C9A8B8172}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D08805B8-0780-47AD-985A-EB6CE71BB593}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-9870" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Branch name</t>
   </si>
@@ -85,6 +85,12 @@
   </si>
   <si>
     <t>Create Map Component</t>
+  </si>
+  <si>
+    <t>#100009</t>
+  </si>
+  <si>
+    <t>CreateMain Page</t>
   </si>
 </sst>
 </file>
@@ -408,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,6 +506,14 @@
         <v>19</v>
       </c>
     </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add simple map to TrackDriver component
</commit_message>
<xml_diff>
--- a/doc/plan.xlsx
+++ b/doc/plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NAUKA_IT\JAVA\TruckPark-server_side\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D08805B8-0780-47AD-985A-EB6CE71BB593}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D278DCA-77A5-4D5C-8C7A-FA74EA7AFAB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-9870" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Branch name</t>
   </si>
@@ -90,7 +90,13 @@
     <t>#100009</t>
   </si>
   <si>
-    <t>CreateMain Page</t>
+    <t>#100010</t>
+  </si>
+  <si>
+    <t>Create Main Page</t>
+  </si>
+  <si>
+    <t>Create Driver Tracking module</t>
   </si>
 </sst>
 </file>
@@ -414,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,7 +517,15 @@
         <v>20</v>
       </c>
       <c r="B11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add basic design, table and buttons to DriverOverview Component
</commit_message>
<xml_diff>
--- a/doc/plan.xlsx
+++ b/doc/plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NAUKA_IT\JAVA\TruckPark-server_side\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D278DCA-77A5-4D5C-8C7A-FA74EA7AFAB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2125E3A5-BB5C-4A78-AD10-E58DFF2B9C34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-9870" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Branch name</t>
   </si>
@@ -96,7 +96,13 @@
     <t>Create Main Page</t>
   </si>
   <si>
-    <t>Create Driver Tracking module</t>
+    <t>#100011</t>
+  </si>
+  <si>
+    <t>Create Driver preview module</t>
+  </si>
+  <si>
+    <t>Create Map Previev Component</t>
   </si>
 </sst>
 </file>
@@ -420,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,7 +531,15 @@
         <v>21</v>
       </c>
       <c r="B12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add TruckPreviev Component and delete diver management component.
</commit_message>
<xml_diff>
--- a/doc/plan.xlsx
+++ b/doc/plan.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NAUKA_IT\JAVA\TruckPark-server_side\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2125E3A5-BB5C-4A78-AD10-E58DFF2B9C34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2EEAE1C-F351-4EE5-A751-B1FEB10DECA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-9870" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Branch name</t>
   </si>
@@ -103,6 +104,12 @@
   </si>
   <si>
     <t>Create Map Previev Component</t>
+  </si>
+  <si>
+    <t>#100012</t>
+  </si>
+  <si>
+    <t>Create Truck preview module</t>
   </si>
 </sst>
 </file>
@@ -426,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,6 +549,14 @@
         <v>24</v>
       </c>
     </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Mappers refactorization - delete ModelMapper
</commit_message>
<xml_diff>
--- a/doc/plan.xlsx
+++ b/doc/plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NAUKA_IT\JAVA\TruckPark-server_side\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2EEAE1C-F351-4EE5-A751-B1FEB10DECA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{403AF5A1-DD40-4612-9BDA-ACEF30FB94B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Branch name</t>
   </si>
@@ -110,6 +109,12 @@
   </si>
   <si>
     <t>Create Truck preview module</t>
+  </si>
+  <si>
+    <t>#100013</t>
+  </si>
+  <si>
+    <t>Pom cleaning and complete README.ME file</t>
   </si>
 </sst>
 </file>
@@ -433,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,6 +562,14 @@
         <v>27</v>
       </c>
     </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Create a prototype of authentication and authorization system
</commit_message>
<xml_diff>
--- a/doc/plan.xlsx
+++ b/doc/plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NAUKA_IT\JAVA\TruckPark-server_side\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{403AF5A1-DD40-4612-9BDA-ACEF30FB94B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CECAB90D-484F-4396-A17D-57290D5EAE67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Branch name</t>
   </si>
@@ -114,7 +114,13 @@
     <t>#100013</t>
   </si>
   <si>
-    <t>Pom cleaning and complete README.ME file</t>
+    <t>Pom cleaning , add completed featuers to README.ME file, some refactorization</t>
+  </si>
+  <si>
+    <t>#100014</t>
+  </si>
+  <si>
+    <t>Add keycloak logging based on docker container</t>
   </si>
 </sst>
 </file>
@@ -438,19 +444,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="44.85546875" customWidth="1"/>
+    <col min="1" max="1" width="12.88671875" customWidth="1"/>
+    <col min="2" max="2" width="44.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -458,7 +464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -466,7 +472,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -474,7 +480,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -482,7 +488,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -490,7 +496,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -498,7 +504,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -506,7 +512,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -514,7 +520,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -522,7 +528,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -530,7 +536,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -538,7 +544,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -546,7 +552,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -554,7 +560,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -562,12 +568,20 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>28</v>
       </c>
       <c r="B15" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>